<commit_message>
added test using basic dita rule to see if it can correctly test several different illegal and legal <ol> scenarios; passing most tests, but getting 2 false positives
</commit_message>
<xml_diff>
--- a/xml/Dita 1.3 Manual Spec Conversion.xlsx
+++ b/xml/Dita 1.3 Manual Spec Conversion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="105">
   <si>
     <t>initial</t>
   </si>
@@ -34,6 +34,9 @@
     <t>attributes rule</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t>symbol guide</t>
   </si>
   <si>
@@ -52,6 +55,28 @@
     <t>(&lt;data&gt; | &lt;sort-as&gt; | &lt;data-about&gt;)*, &lt;li&gt;+</t>
   </si>
   <si>
+    <t>   compact (yes|no|-dita-use-conref-target) #IMPLIED
+    spectitle CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/ol "</t>
+  </si>
+  <si>
     <t>*</t>
   </si>
   <si>
@@ -67,6 +92,33 @@
     <t>ul</t>
   </si>
   <si>
+    <t xml:space="preserve">
+    compact (yes|no|-dita-use-conref-target) #IMPLIED
+    spectitle CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    feature CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/ul "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/ul.html</t>
+  </si>
+  <si>
     <t>+</t>
   </si>
   <si>
@@ -76,16 +128,573 @@
     <t>instructions</t>
   </si>
   <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>entry</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade | term | xref | cite | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | p | lq | note | dl | parml | ul | ol | sl | pre | codeblock | msgblock | screen | lines | fig | syntaxdiagram | imagemap | image | object | draft-comment | required-cleanup | fn | indextermref | indexterm | data | data-about | foreign | unknown)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    colname NMTOKEN #IMPLIED
+    namest NMTOKEN #IMPLIED
+    nameend NMTOKEN #IMPLIED
+    morerows NMTOKEN #IMPLIED
+    colsep NMTOKEN #IMPLIED
+    rowsep NMTOKEN #IMPLIED
+    align (left|right|center|justify|char|-dita-use-conref-target) #IMPLIED
+    char CDATA #IMPLIED
+    charoff NMTOKEN #IMPLIED
+    valign (top|middle|bottom|-dita-use-conref-target) #IMPLIED
+    base CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/entry "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/entry.html</t>
+  </si>
+  <si>
     <t>?</t>
   </si>
   <si>
     <t>zero or one</t>
   </si>
   <si>
+    <t>colspec</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    colnum NMTOKEN #IMPLIED
+    colname NMTOKEN #IMPLIED
+    colwidth CDATA #IMPLIED
+    colsep NMTOKEN #IMPLIED
+    rowsep NMTOKEN #IMPLIED
+    align (left|right|center|justify|char|-dita-use-conref-target) #IMPLIED
+    char CDATA #IMPLIED
+    charoff NMTOKEN #IMPLIED
+    base CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/colspec "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/colspec.html</t>
+  </si>
+  <si>
     <t>|</t>
   </si>
   <si>
     <t>or</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade | term | xref | xref-external | cite | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | lq | note | dl | parml | ul | ol | sl | pre | codeblock | msgblock | screen | lines | fig | syntaxdiagram | imagemap | image | object | table | simpletable | draft-comment | required-cleanup | fn | indextermref | indexterm | data | data-about | foreign | unknown | dataref)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/p "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/p.html</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>(entry+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    rowsep NMTOKEN #IMPLIED
+    valign (top|middle|bottom|-dita-use-conref-target) #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/row "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/row.html</t>
+  </si>
+  <si>
+    <t>sli</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade | term | xref | cite | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | image | draft-comment | required-cleanup | fn | indextermref | indexterm | data | data-about | foreign | unknown)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/sli "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/sli.html</t>
+  </si>
+  <si>
+    <t>xref</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade | term | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | image | data | data-about | foreign | unknown | desc)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    href CDATA #IMPLIED
+    keyref CDATA #IMPLIED
+    type CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    feature CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    format CDATA #IMPLIED
+    scope (local|peer|external|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/xref "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/xref.html</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> keyref CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    feature CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/ph "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/ph.html</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade | active-low | completed | day | month | year | change-summary | term | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | image | data | changehistory | edited | person | data-about | foreign | unknown)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    base CDATA #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/title "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/title.html</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade | term | xref | cite | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | p | lq | note | dl | parml | ul | ol | sl | pre | codeblock | msgblock | screen | lines | fig | syntaxdiagram | imagemap | image | object | table | simpletable | title | draft-comment | required-cleanup | fn | indextermref | indexterm | data | data-about | foreign | unknown)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    spectitle CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/section "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/section.html</t>
+  </si>
+  <si>
+    <t>tgroup</t>
+  </si>
+  <si>
+    <t>((colspec*, thead?, tbody))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    cols NMTOKEN #REQUIRED
+    colsep NMTOKEN #IMPLIED
+    rowsep NMTOKEN #IMPLIED
+    align (left|right|center|justify|char|-dita-use-conref-target) #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/tgroup "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/tgroup.html</t>
+  </si>
+  <si>
+    <t>tbody</t>
+  </si>
+  <si>
+    <t>(row+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    valign (top|middle|bottom|-dita-use-conref-target) #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/tbody "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/tbody.html</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>(((title?, desc?)?, tgroup+))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    frame (top|bottom|topbot|all|sides|none|-dita-use-conref-target) #IMPLIED
+    colsep NMTOKEN #IMPLIED
+    rowsep NMTOKEN #IMPLIED
+    pgwide NMTOKEN #IMPLIED
+    rowheader (firstcol|norowheader|-dita-use-conref-target) #IMPLIED
+    scale (50|60|70|80|90|100|110|120|140|160|180|200|-dita-use-conref-target) #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/table "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/table.html</t>
+  </si>
+  <si>
+    <t>thead</t>
+  </si>
+  <si>
+    <t>thead
+    valign (top|middle|bottom|-dita-use-conref-target) #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/thead "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/thead.html</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>(sli+)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    compact (yes|no|-dita-use-conref-target) #IMPLIED
+    spectitle CDATA #IMPLIED
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/sl "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/sl.html</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>((title, titlealts?, (shortdesc| abstract)?, prolog?, body?, related-links?, topic*))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    id ID #REQUIRED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xmlns:ditaarch CDATA #FIXED "http://dita.oasis-open.org/architecture/2005/"
+    ditaarch:DITAArchVersion CDATA "1.1"
+    domains CDATA "(topic ui-d)  (topic hi-d)  (topic pr-d)  (topic sw-d) (topic ut-d)  (topic indexing-d)  (topic revhistoryDomain-d)  (topic sidscDomain-d)  a(props  feature)"
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/topic "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/topic.html</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>((p| lq| note| dl| parml| ul| ol| sl| pre| codeblock| msgblock| screen| lines| fig| syntaxdiagram| imagemap| image| object| table| simpletable| required-cleanup| data| data-about| foreign| unknown| section| example)*)&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/body "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/body.html</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>(#PCDATA | ph | codeph | synph | filepath | msgph | userinput | systemoutput | b | u | i | tt | sup | sub | uicontrol | menucascade| term | xref | cite | q | boolean | state | keyword | option | parmname | apiname | cmdname | msgnum | varname | wintitle | tm | p | lq | note | dl | parml | ul | ol | sl | pre | codeblock | msgblock | screen | lines | fig | syntaxdiagram | imagemap | image | object | table | simpletable | itemgroup | draft-comment | required-cleanup | fn | indextermref | indexterm | data | data-about | foreign | unknown)*&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    id NMTOKEN #IMPLIED
+    conref CDATA #IMPLIED
+    props CDATA #IMPLIED
+    platform CDATA #IMPLIED
+    product CDATA #IMPLIED
+    audience CDATA #IMPLIED
+    otherprops CDATA #IMPLIED
+    base CDATA #IMPLIED
+    importance (obsolete|deprecated|optional|default|low|normal|high|recommended|required|urgent|-dita-use-conref-target) #IMPLIED
+    rev CDATA #IMPLIED
+    status (new|changed|deleted|unchanged|-dita-use-conref-target) #IMPLIED
+    translate (yes|no|-dita-use-conref-target) #IMPLIED
+    xml:lang NMTOKEN #IMPLIED
+    dir (ltr|rtl|lro|rlo|-dita-use-conref-target) #IMPLIED
+    outputclass CDATA #IMPLIED
+    xtrc CDATA #IMPLIED
+    xtrf CDATA #IMPLIED
+    class CDATA "- topic/li "</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/li.html</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/note.html</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/data.html</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/i.html</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/b.html</t>
+  </si>
+  <si>
+    <t>data-about</t>
+  </si>
+  <si>
+    <t>http://docs.oasis-open.org/dita/dita/v1.3/os/part3-all-inclusive/langRef/base/data-about.html</t>
   </si>
 </sst>
 </file>
@@ -138,10 +747,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,102 +1077,580 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="37.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="37.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="95.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="375">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="409.6">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="330">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="270">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="360">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="390">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="360">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="409.6">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="375">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="150">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="375">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="409.6">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="375">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="409.6">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="375">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="390">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="409.6">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="360">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="360">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified rule mechanism to only apply applicable rules also generates null patterns for missing required attributes/children; general code improvements and docs; massive performance boost; grammar now loads from memory when possible History and Grammar sub components now use standardized def initialize to allow custom argument behavior
</commit_message>
<xml_diff>
--- a/xml/Dita 1.3 Manual Spec Conversion.xlsx
+++ b/xml/Dita 1.3 Manual Spec Conversion.xlsx
@@ -3,13 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b33791\RubymineProjects\Dux\xml\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -700,8 +705,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,23 +861,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -908,23 +896,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1079,9 +1050,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="2"/>
     <col min="4" max="4" width="9.140625" style="3"/>
@@ -1090,7 +1063,7 @@
     <col min="7" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1119,425 +1092,425 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="375">
+    <row r="2" spans="1:11" ht="375" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="330" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="409.6">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:11" ht="360" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="330">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
+    <row r="5" spans="1:11" ht="330" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="270">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="3" t="s">
+    <row r="6" spans="1:11" ht="270" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="360">
-      <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    <row r="7" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="390">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    <row r="8" spans="1:11" ht="345" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="360">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
+    <row r="9" spans="1:11" ht="315" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="409.6">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="3" t="s">
+    <row r="10" spans="1:11" ht="405" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="375">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    <row r="11" spans="1:11" ht="330" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="150">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
+    <row r="12" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="375">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
+    <row r="13" spans="1:11" ht="330" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="409.6">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="3" t="s">
+    <row r="14" spans="1:11" ht="375" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="375">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3" t="s">
+    <row r="15" spans="1:11" ht="330" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="409.6">
-      <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
+    <row r="16" spans="1:11" ht="405" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="375">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
+    <row r="17" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="390">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
+    <row r="18" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="409.6">
-      <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="360">
+    <row r="19" spans="1:7" ht="315" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1560,7 +1533,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="360">
+    <row r="20" spans="1:7" ht="315" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1583,7 +1556,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1597,7 +1570,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1611,7 +1584,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1625,7 +1598,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1639,7 +1612,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1655,9 +1628,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="K2" r:id="rId2"/>
-    <hyperlink ref="K3" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>